<commit_message>
Se ha adaptado la hoja excel con los ODS relacionados a mi proyecto.
</commit_message>
<xml_diff>
--- a/ODS.xlsx
+++ b/ODS.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalva\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA63402-0449-4F35-A1FA-83C6044E4AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{144071DE-BB33-4985-B47F-836A21E985D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="924" yWindow="2232" windowWidth="15312" windowHeight="14304" xr2:uid="{7355BA2D-9C48-415E-81BC-138F08BEB434}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,80 +38,80 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
+    <t xml:space="preserve">ODS </t>
+  </si>
+  <si>
+    <t>No procede (0)</t>
+  </si>
+  <si>
+    <t>Bajo (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medio (2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alto (3) </t>
+  </si>
+  <si>
     <t>1 Fin de la Pobreza</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>2 Hambre cero</t>
   </si>
   <si>
     <t>3 Salud y Bienestar</t>
   </si>
   <si>
+    <t>4 Educación de calidad</t>
+  </si>
+  <si>
+    <t>5 Igualdad de género</t>
+  </si>
+  <si>
     <t>6 Agua limpia y saneamiento</t>
   </si>
   <si>
+    <t>7 Energía Asequible y no contaminante</t>
+  </si>
+  <si>
+    <t>8 Trabajo decente y crecimiento económico</t>
+  </si>
+  <si>
+    <t>9 Industria, Innovación e Infraestructuras</t>
+  </si>
+  <si>
+    <t>10 Reducción de las desigualdades</t>
+  </si>
+  <si>
     <t>11 Ciudades y comunidades sostenibles</t>
   </si>
   <si>
+    <t>12 Producción y consumo sostenibles</t>
+  </si>
+  <si>
+    <t>13 Acción por el clima</t>
+  </si>
+  <si>
     <t>14 Vida submarina</t>
   </si>
   <si>
     <t>15 Vida de ecosistemas terrestres</t>
   </si>
   <si>
+    <t>16 Paz, justicia e instituciones sólidas</t>
+  </si>
+  <si>
     <t>17 Alianzas para lograr objetivos</t>
-  </si>
-  <si>
-    <t>4 Educación de calidad</t>
-  </si>
-  <si>
-    <t>5 Igualdad de género</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODS </t>
-  </si>
-  <si>
-    <t>7 Energía Asequible y no contaminante</t>
-  </si>
-  <si>
-    <t>8 Trabajo decente y crecimiento económico</t>
-  </si>
-  <si>
-    <t>9 Industria, Innovación e Infraestructuras</t>
-  </si>
-  <si>
-    <t>10 Reducción de las desigualdades</t>
-  </si>
-  <si>
-    <t>12 Producción y consumo sostenibles</t>
-  </si>
-  <si>
-    <t>13 Acción por el clima</t>
-  </si>
-  <si>
-    <t>16 Paz, justicia e instituciones sólidas</t>
-  </si>
-  <si>
-    <t>No procede (0)</t>
-  </si>
-  <si>
-    <t>Bajo (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medio (2) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alto (3) </t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,165 +479,165 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>